<commit_message>
New Drugs from Dr. Kalpas
</commit_message>
<xml_diff>
--- a/Active_Not_Found.xlsx
+++ b/Active_Not_Found.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hm/Documents/opioid_list/opioid_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCB9530-2913-0B42-802B-A47D8FAF18B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05245DC6-B594-174E-B185-D75E1F21F6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="110">
   <si>
     <t>rxcui</t>
   </si>
@@ -55,21 +55,6 @@
     <t>remappedDate</t>
   </si>
   <si>
-    <t>1154667</t>
-  </si>
-  <si>
-    <t>1154668</t>
-  </si>
-  <si>
-    <t>1154669</t>
-  </si>
-  <si>
-    <t>1161354</t>
-  </si>
-  <si>
-    <t>1161355</t>
-  </si>
-  <si>
     <t>1165327</t>
   </si>
   <si>
@@ -85,39 +70,12 @@
     <t>1176518</t>
   </si>
   <si>
-    <t>1179650</t>
-  </si>
-  <si>
-    <t>1179651</t>
-  </si>
-  <si>
-    <t>1179656</t>
-  </si>
-  <si>
-    <t>1179657</t>
-  </si>
-  <si>
-    <t>1190568</t>
-  </si>
-  <si>
-    <t>1190572</t>
-  </si>
-  <si>
-    <t>1190641</t>
-  </si>
-  <si>
-    <t>1190646</t>
-  </si>
-  <si>
     <t>1250685</t>
   </si>
   <si>
     <t>1250693</t>
   </si>
   <si>
-    <t>200240</t>
-  </si>
-  <si>
     <t>1307713</t>
   </si>
   <si>
@@ -193,9 +151,6 @@
     <t>1811764</t>
   </si>
   <si>
-    <t>215451</t>
-  </si>
-  <si>
     <t>221074</t>
   </si>
   <si>
@@ -205,21 +160,9 @@
     <t>314517</t>
   </si>
   <si>
-    <t>32926</t>
-  </si>
-  <si>
-    <t>402519</t>
-  </si>
-  <si>
     <t>544581</t>
   </si>
   <si>
-    <t>6377</t>
-  </si>
-  <si>
-    <t>690713</t>
-  </si>
-  <si>
     <t>71225</t>
   </si>
   <si>
@@ -229,21 +172,6 @@
     <t>42347</t>
   </si>
   <si>
-    <t>atropine / diphenoxylate Oral Liquid Product</t>
-  </si>
-  <si>
-    <t>atropine / diphenoxylate Oral Product</t>
-  </si>
-  <si>
-    <t>atropine / diphenoxylate Pill</t>
-  </si>
-  <si>
-    <t>paregoric Oral Liquid Product</t>
-  </si>
-  <si>
-    <t>paregoric Oral Product</t>
-  </si>
-  <si>
     <t>loperamide Oral Liquid Product</t>
   </si>
   <si>
@@ -259,39 +187,12 @@
     <t>Diamode Oral Product</t>
   </si>
   <si>
-    <t>Lomotil Oral Product</t>
-  </si>
-  <si>
-    <t>Lomotil Pill</t>
-  </si>
-  <si>
-    <t>Lonox Oral Product</t>
-  </si>
-  <si>
-    <t>Lonox Pill</t>
-  </si>
-  <si>
-    <t>atropine sulfate 0.005 MG/ML / diphenoxylate hydrochloride 0.5 MG/ML Oral Solution</t>
-  </si>
-  <si>
-    <t>atropine sulfate 0.025 MG / diphenoxylate hydrochloride 2.5 MG Oral Tablet</t>
-  </si>
-  <si>
-    <t>atropine sulfate 0.025 MG / diphenoxylate hydrochloride 2.5 MG Oral Tablet [Lomotil]</t>
-  </si>
-  <si>
-    <t>atropine sulfate 0.025 MG / diphenoxylate hydrochloride 2.5 MG Oral Tablet [Lonox]</t>
-  </si>
-  <si>
     <t>loperamide hydrochloride 0.133 MG/ML Oral Suspension</t>
   </si>
   <si>
     <t>loperamide hydrochloride 0.133 MG/ML Oral Suspension [Imodium]</t>
   </si>
   <si>
-    <t>paregoric 0.4 MG/ML Oral Solution</t>
-  </si>
-  <si>
     <t>Kalopanax septemlobus bark extract</t>
   </si>
   <si>
@@ -367,9 +268,6 @@
     <t>Atropa belladonna flowering top extract</t>
   </si>
   <si>
-    <t>aspirin / oxycodone hydrochloride / oxycodone terephthalate</t>
-  </si>
-  <si>
     <t>chlorpheniramine polistirex</t>
   </si>
   <si>
@@ -379,21 +277,9 @@
     <t>belladonna leaf extract</t>
   </si>
   <si>
-    <t>paregoric</t>
-  </si>
-  <si>
-    <t>levopropoxyphene napsylate</t>
-  </si>
-  <si>
     <t>Apokyn</t>
   </si>
   <si>
-    <t>levopropoxyphene</t>
-  </si>
-  <si>
-    <t>kaolin / paregoric / pectin</t>
-  </si>
-  <si>
     <t>apomorphine hydrochloride</t>
   </si>
   <si>
@@ -436,18 +322,15 @@
     <t>102011</t>
   </si>
   <si>
-    <t>112011</t>
-  </si>
-  <si>
     <t>052012</t>
   </si>
   <si>
+    <t>102012</t>
+  </si>
+  <si>
     <t>042005</t>
   </si>
   <si>
-    <t>102012</t>
-  </si>
-  <si>
     <t>092010</t>
   </si>
   <si>
@@ -461,9 +344,6 @@
   </si>
   <si>
     <t>092005</t>
-  </si>
-  <si>
-    <t>042007</t>
   </si>
   <si>
     <t>YES</t>
@@ -871,16 +751,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
@@ -929,1515 +809,1021 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="H2" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I2" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" t="s">
         <v>109</v>
-      </c>
-      <c r="C3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" t="s">
-        <v>136</v>
-      </c>
-      <c r="F3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" t="s">
-        <v>148</v>
-      </c>
-      <c r="I3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="H4" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I4" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="H5" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I5" t="s">
-        <v>142</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F6" t="s">
-        <v>145</v>
+        <v>104</v>
       </c>
       <c r="H6" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I6" t="s">
-        <v>145</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="H7" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I7" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E8" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F8" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="H8" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I8" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E9" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F9" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="H9" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I9" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E10" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F10" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="H10" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I10" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F11" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="H11" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I11" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E12" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F12" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="H12" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I12" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E13" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="H13" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I13" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E14" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="H14" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I14" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E15" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F15" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="H15" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I15" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>130</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E16" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F16" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="H16" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I16" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E17" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F17" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="H17" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I17" t="s">
-        <v>149</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E18" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F18" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="H18" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I18" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="D19" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F19" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="H19" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I19" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E20" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F20" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="H20" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I20" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E21" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F21" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="H21" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I21" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E22" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F22" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="H22" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I22" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E23" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F23" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="H23" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I23" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F24" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="H24" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I24" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E25" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F25" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="H25" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I25" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D26" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E26" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F26" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="H26" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I26" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E27" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F27" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="H27" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I27" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F28" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="H28" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I28" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E29" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F29" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="H29" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I29" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
-        <v>132</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E30" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F30" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="H30" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I30" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E31" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F31" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="H31" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I31" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" t="s">
         <v>99</v>
       </c>
-      <c r="C32" t="s">
-        <v>132</v>
-      </c>
-      <c r="D32" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" t="s">
-        <v>136</v>
-      </c>
-      <c r="F32" t="s">
-        <v>142</v>
-      </c>
       <c r="H32" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I32" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>90</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E33" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F33" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="H33" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I33" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D34" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E34" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F34" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="H34" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I34" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E35" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F35" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="H35" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I35" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>96</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E36" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F36" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
       <c r="H36" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I36" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>133</v>
+        <v>91</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E37" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F37" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="H37" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I37" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E38" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F38" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="H38" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I38" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s">
         <v>50</v>
       </c>
-      <c r="B39" t="s">
-        <v>108</v>
-      </c>
       <c r="C39" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F39" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="H39" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I39" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="E40" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F40" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="H40" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="I40" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" t="s">
-        <v>128</v>
-      </c>
-      <c r="D41" t="s">
-        <v>135</v>
-      </c>
-      <c r="E41" t="s">
-        <v>136</v>
-      </c>
-      <c r="F41" t="s">
-        <v>137</v>
-      </c>
-      <c r="H41" t="s">
-        <v>148</v>
-      </c>
-      <c r="I41" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" t="s">
-        <v>131</v>
-      </c>
-      <c r="D42" t="s">
-        <v>135</v>
-      </c>
-      <c r="E42" t="s">
-        <v>136</v>
-      </c>
-      <c r="F42" t="s">
-        <v>141</v>
-      </c>
-      <c r="H42" t="s">
-        <v>148</v>
-      </c>
-      <c r="I42" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D43" t="s">
-        <v>135</v>
-      </c>
-      <c r="E43" t="s">
-        <v>136</v>
-      </c>
-      <c r="F43" t="s">
-        <v>147</v>
-      </c>
-      <c r="H43" t="s">
-        <v>148</v>
-      </c>
-      <c r="I43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>64</v>
-      </c>
-      <c r="B44" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D44" t="s">
-        <v>135</v>
-      </c>
-      <c r="E44" t="s">
-        <v>136</v>
-      </c>
-      <c r="F44" t="s">
-        <v>140</v>
-      </c>
-      <c r="H44" t="s">
-        <v>148</v>
-      </c>
-      <c r="I44" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B45" t="s">
-        <v>120</v>
-      </c>
-      <c r="C45" t="s">
-        <v>133</v>
-      </c>
-      <c r="D45" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" t="s">
-        <v>136</v>
-      </c>
-      <c r="F45" t="s">
-        <v>140</v>
-      </c>
-      <c r="H45" t="s">
-        <v>148</v>
-      </c>
-      <c r="I45" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" t="s">
-        <v>117</v>
-      </c>
-      <c r="C46" t="s">
-        <v>131</v>
-      </c>
-      <c r="D46" t="s">
-        <v>135</v>
-      </c>
-      <c r="E46" t="s">
-        <v>136</v>
-      </c>
-      <c r="F46" t="s">
-        <v>140</v>
-      </c>
-      <c r="H46" t="s">
-        <v>148</v>
-      </c>
-      <c r="I46" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>21</v>
-      </c>
-      <c r="B47" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47" t="s">
-        <v>128</v>
-      </c>
-      <c r="D47" t="s">
-        <v>135</v>
-      </c>
-      <c r="E47" t="s">
-        <v>136</v>
-      </c>
-      <c r="F47" t="s">
-        <v>137</v>
-      </c>
-      <c r="H47" t="s">
-        <v>148</v>
-      </c>
-      <c r="I47" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" t="s">
-        <v>128</v>
-      </c>
-      <c r="D48" t="s">
-        <v>135</v>
-      </c>
-      <c r="E48" t="s">
-        <v>136</v>
-      </c>
-      <c r="F48" t="s">
-        <v>137</v>
-      </c>
-      <c r="H48" t="s">
-        <v>148</v>
-      </c>
-      <c r="I48" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>23</v>
-      </c>
-      <c r="B49" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" t="s">
-        <v>128</v>
-      </c>
-      <c r="D49" t="s">
-        <v>135</v>
-      </c>
-      <c r="E49" t="s">
-        <v>136</v>
-      </c>
-      <c r="F49" t="s">
-        <v>137</v>
-      </c>
-      <c r="H49" t="s">
-        <v>148</v>
-      </c>
-      <c r="I49" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" t="s">
-        <v>82</v>
-      </c>
-      <c r="C50" t="s">
-        <v>128</v>
-      </c>
-      <c r="D50" t="s">
-        <v>135</v>
-      </c>
-      <c r="E50" t="s">
-        <v>136</v>
-      </c>
-      <c r="F50" t="s">
-        <v>137</v>
-      </c>
-      <c r="H50" t="s">
-        <v>148</v>
-      </c>
-      <c r="I50" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>33</v>
-      </c>
-      <c r="B51" t="s">
-        <v>91</v>
-      </c>
-      <c r="C51" t="s">
-        <v>131</v>
-      </c>
-      <c r="D51" t="s">
-        <v>135</v>
-      </c>
-      <c r="E51" t="s">
-        <v>136</v>
-      </c>
-      <c r="F51" t="s">
-        <v>140</v>
-      </c>
-      <c r="H51" t="s">
-        <v>148</v>
-      </c>
-      <c r="I51" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" t="s">
-        <v>87</v>
-      </c>
-      <c r="C52" t="s">
-        <v>129</v>
-      </c>
-      <c r="D52" t="s">
-        <v>135</v>
-      </c>
-      <c r="E52" t="s">
-        <v>136</v>
-      </c>
-      <c r="F52" t="s">
-        <v>139</v>
-      </c>
-      <c r="H52" t="s">
-        <v>148</v>
-      </c>
-      <c r="I52" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>30</v>
-      </c>
-      <c r="B53" t="s">
-        <v>88</v>
-      </c>
-      <c r="C53" t="s">
-        <v>130</v>
-      </c>
-      <c r="D53" t="s">
-        <v>135</v>
-      </c>
-      <c r="E53" t="s">
-        <v>136</v>
-      </c>
-      <c r="F53" t="s">
-        <v>139</v>
-      </c>
-      <c r="H53" t="s">
-        <v>148</v>
-      </c>
-      <c r="I53" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>16</v>
-      </c>
-      <c r="B54" t="s">
-        <v>74</v>
-      </c>
-      <c r="C54" t="s">
-        <v>127</v>
-      </c>
-      <c r="D54" t="s">
-        <v>135</v>
-      </c>
-      <c r="E54" t="s">
-        <v>136</v>
-      </c>
-      <c r="F54" t="s">
-        <v>137</v>
-      </c>
-      <c r="H54" t="s">
-        <v>148</v>
-      </c>
-      <c r="I54" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>17</v>
-      </c>
-      <c r="B55" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" t="s">
-        <v>127</v>
-      </c>
-      <c r="D55" t="s">
-        <v>135</v>
-      </c>
-      <c r="E55" t="s">
-        <v>136</v>
-      </c>
-      <c r="F55" t="s">
-        <v>137</v>
-      </c>
-      <c r="H55" t="s">
-        <v>148</v>
-      </c>
-      <c r="I55" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" t="s">
-        <v>119</v>
-      </c>
-      <c r="C56" t="s">
-        <v>131</v>
-      </c>
-      <c r="D56" t="s">
-        <v>135</v>
-      </c>
-      <c r="E56" t="s">
-        <v>136</v>
-      </c>
-      <c r="F56" t="s">
-        <v>140</v>
-      </c>
-      <c r="H56" t="s">
-        <v>148</v>
-      </c>
-      <c r="I56" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>31</v>
-      </c>
-      <c r="B57" t="s">
-        <v>89</v>
-      </c>
-      <c r="C57" t="s">
-        <v>129</v>
-      </c>
-      <c r="D57" t="s">
-        <v>135</v>
-      </c>
-      <c r="E57" t="s">
-        <v>136</v>
-      </c>
-      <c r="F57" t="s">
-        <v>140</v>
-      </c>
-      <c r="H57" t="s">
-        <v>148</v>
-      </c>
-      <c r="I57" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>14</v>
-      </c>
-      <c r="B58" t="s">
-        <v>72</v>
-      </c>
-      <c r="C58" t="s">
-        <v>127</v>
-      </c>
-      <c r="D58" t="s">
-        <v>135</v>
-      </c>
-      <c r="E58" t="s">
-        <v>136</v>
-      </c>
-      <c r="F58" t="s">
-        <v>137</v>
-      </c>
-      <c r="H58" t="s">
-        <v>148</v>
-      </c>
-      <c r="I58" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>15</v>
-      </c>
-      <c r="B59" t="s">
-        <v>73</v>
-      </c>
-      <c r="C59" t="s">
-        <v>127</v>
-      </c>
-      <c r="D59" t="s">
-        <v>135</v>
-      </c>
-      <c r="E59" t="s">
-        <v>136</v>
-      </c>
-      <c r="F59" t="s">
-        <v>137</v>
-      </c>
-      <c r="H59" t="s">
-        <v>148</v>
-      </c>
-      <c r="I59" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K59">
-    <sortCondition ref="B1:B59"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K40">
+    <sortCondition ref="B1:B40"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>